<commit_message>
Fixed pre-primary Special Instructions issue - special instructions are now printed on every label
</commit_message>
<xml_diff>
--- a/tuckshop.xlsx
+++ b/tuckshop.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.whiskin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.whiskin\workspace\tuckshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -120,11 +120,7 @@
     <t>Hot Dog without Sauce, Hot Dog with Sauce, Fresh Corn 1/2 Cob, Slice of Pizza - Vegetarian, Slice of Pizza - Cheese &amp; Tomato</t>
   </si>
   <si>
-    <t>This kid is allergic to a lot of stuff:
-- Lactose
-- Milk
-- Cheese
-- Dust</t>
+    <t>SPECIAL</t>
   </si>
 </sst>
 </file>
@@ -970,9 +966,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="18" max="18" width="52.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>